<commit_message>
sprint 1 almost finished
</commit_message>
<xml_diff>
--- a/planning/planning.xlsx
+++ b/planning/planning.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t xml:space="preserve">open</t>
   </si>
@@ -58,157 +58,163 @@
     <t xml:space="preserve">Progresso</t>
   </si>
   <si>
-    <t xml:space="preserve"> animações básicas de personagem (idle + movimentação)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> animações básicas de 1 monstro (idle + movimentação)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tileset básico (1 dungeon completa - chão, paredes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de scrolling da dungeon</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> uma dungeon básica implementada (sem autogeração ainda)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mecânica básica de movimentação</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação de inputs via mouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mecânica de movimento básico do jogador</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> definição de inicio, fim e próximo andar de uma dungeon</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primeira dungeon com profundidade 3 (início, meio e fim)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação de inputs via touch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> configuração da tela para dispositivos móveis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primeiro deploy pra android</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de atributos do personagem</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mecânica geral do funcionamento dos atibutos e influência de cada atributo na relaização de ações</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sprites de vida, stamina e magia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema básico de vida, stamina e magia (uso de componentes de GUI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mecânica básica de morte do aventureiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de turnos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema básico de ataque (1 arma branca e 1 de fogo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de bloqueio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mecânica de movimento básico do monstro 1 (aleatório bem básico)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA (comportamento) básica do monstro 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de observação de corredor de dungeon (peek system)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> animações para o peek system</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> adição de explosivos</t>
+    <t xml:space="preserve">animações básicas de personagem (idle + movimentação)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animações básicas de 1 monstro (idle + movimentação)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tileset básico (1 dungeon completa - chão, paredes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de scrolling da dungeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uma dungeon básica implementada (sem autogeração ainda)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mecânica básica de movimentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação de inputs via mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mecânica de movimento básico do jogador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alteração de paleta de cores dos sprites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estudar ferramenta de gerenciamento de times clubhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definição de inicio, fim e próximo andar de uma dungeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primeira dungeon com profundidade 3 (início, meio e fim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação de inputs via touch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configuração da tela para dispositivos móveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primeiro deploy pra android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de atributos do personagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mecânica geral do funcionamento dos atibutos e influência de cada atributo na relaização de ações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprites de vida, stamina e magia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema básico de vida, stamina e magia (uso de componentes de GUI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mecânica básica de morte do aventureiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de turnos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema básico de ataque (1 arma branca e 1 de fogo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de bloqueio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mecânica de movimento básico do monstro 1 (aleatório bem básico)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IA (comportamento) básica do monstro 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de observação de corredor de dungeon (peek system)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animações para o peek system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adição de explosivos</t>
   </si>
   <si>
     <t xml:space="preserve">impacto dos explosivos no cenário (cenário parcialmente detrutível?)</t>
   </si>
   <si>
-    <t xml:space="preserve"> sprites (botões, setas, tiles, etc) e cenário da guilda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema da guilda - recrutamento de novos aventureiros (1 dentre 3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema da guilda - escolha de dungeons (1 dentre 3) sem geração aleatória ainda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema completo de morte de um aventureiro (morreu? recruta outro)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de loot + inventário</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de save (Dungeon + Personagem + Guilda)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema monetário da guilda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de espólios da guilda (baú da guilda para guardar os itens que os jogadores desejarem)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> permitir mover item do aventureiro para os espólios da guilda e vice-versa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cosmetics - 3 tipos de cabelo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 sets completo de armadura leve (4 peças - helmo, braçadeiras, peitoral e pernas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de composição de sprites (pesonagem + cabelo + armadura são compostos via sprites distintos no jogo -&gt; máxima reusabilidade)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sprites do segundo monstro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação do sistema de equip load</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mais 2 sets completos de armadura: média e pesada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema da guilda - estoque de aventureiros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação de mecânica do monstro 2 (golpes + IA + atributos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 sprites de monstros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação da mecânica dos 3 monstros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sprites do primeiro chefão</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sistema de geração aleatória de dungeons - parte 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sprites da tela inicial do jogo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> implementação de 3 arquivos de jogos diferentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> menu principal (start game, continue, load, quit)</t>
+    <t xml:space="preserve">sprites (botões, setas, tiles, etc) e cenário da guilda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema da guilda - recrutamento de novos aventureiros (1 dentre 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema da guilda - escolha de dungeons (1 dentre 3) sem geração aleatória ainda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema completo de morte de um aventureiro (morreu? recruta outro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de loot + inventário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de save (Dungeon + Personagem + Guilda)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema monetário da guilda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de espólios da guilda (baú da guilda para guardar os itens que os jogadores desejarem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permitir mover item do aventureiro para os espólios da guilda e vice-versa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosmetics - 3 tipos de cabelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 sets completo de armadura leve (4 peças - helmo, braçadeiras, peitoral e pernas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de composição de sprites (pesonagem + cabelo + armadura são compostos via sprites distintos no jogo -&gt; máxima reusabilidade)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprites do segundo monstro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação do sistema de equip load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mais 2 sets completos de armadura: média e pesada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema da guilda - estoque de aventureiros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação de mecânica do monstro 2 (golpes + IA + atributos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 sprites de monstros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação da mecânica dos 3 monstros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprites do primeiro chefão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema de geração aleatória de dungeons - parte 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprites da tela inicial do jogo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação de 3 arquivos de jogos diferentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu principal (start game, continue, load, quit)</t>
   </si>
 </sst>
 </file>
@@ -292,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,6 +324,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,7 +398,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,25 +428,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -471,7 +481,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,13 +511,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -542,7 +552,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,13 +582,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -613,7 +623,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,19 +653,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -687,10 +697,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -810,14 +820,33 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <f aca="false">SUM(A3:A10)</f>
-        <v>26</v>
+      <c r="A11" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <f aca="false">SUM(A3:A12)</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:C10" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:C11" type="list">
       <formula1>conf!$A$1:$A$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -840,7 +869,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -873,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -882,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -891,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -900,7 +929,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -909,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -944,7 +973,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -977,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -986,7 +1015,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -995,7 +1024,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1004,7 +1033,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1013,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1048,7 +1077,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1081,7 +1110,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -1090,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -1099,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1108,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1143,7 +1172,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1176,7 +1205,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -1185,7 +1214,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -1194,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1203,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1212,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1247,7 +1276,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1277,31 +1306,31 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1336,7 +1365,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1366,25 +1395,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1419,7 +1448,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1449,25 +1478,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6"/>
     </row>

</xml_diff>